<commit_message>
Added the report of create operation
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Test_cases.xlsx
+++ b/cypress/fixtures/Test_cases.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>url</t>
   </si>
@@ -29,7 +29,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>http://testapp.corporate.com/PFS_4.7.2_PL/Account/Login.aspx</t>
+    <t>http://testapp.corporate.com/PFS_4.7.2_PL/Account/Login.aspx/</t>
   </si>
   <si>
     <t>rmuser</t>
@@ -56,7 +56,7 @@
     <t>boardplan</t>
   </si>
   <si>
-    <t>Delete 5</t>
+    <t>Delete 9</t>
   </si>
   <si>
     <t>yes</t>
@@ -65,10 +65,16 @@
     <t>no</t>
   </si>
   <si>
+    <t>Delete 100</t>
+  </si>
+  <si>
+    <t>Delete 101</t>
+  </si>
+  <si>
     <t>cdate</t>
   </si>
   <si>
-    <t>Delete 4</t>
+    <t>Delete 7</t>
   </si>
   <si>
     <t>Demo1 Cycle</t>
@@ -82,8 +88,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
@@ -130,6 +136,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -138,15 +173,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,26 +190,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,6 +212,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -207,38 +227,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,21 +266,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,187 +281,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,15 +472,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,6 +486,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,13 +514,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,32 +556,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,15 +577,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -589,130 +595,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1093,7 +1099,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Surya@123" tooltip="mailto:Surya@123"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://testapp.corporate.com/PFS_4.7.2_PL/Account/Login.aspx" tooltip="http://testapp.corporate.com/PFS_4.9.0_PL/Account/Login.aspx"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://testapp.corporate.com/PFS_4.7.2_PL/Account/Login.aspx/" tooltip="http://testapp.corporate.com/PFS_4.7.2_PL/Account/Login.aspx/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1106,7 +1112,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1139,13 +1145,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="3">
-        <v>44649</v>
+        <v>44828</v>
       </c>
       <c r="C2" s="3">
-        <v>44926</v>
+        <v>45284</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -1154,13 +1160,45 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44649</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45290</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44649</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45290</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="3"/>
@@ -1182,7 +1220,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1192,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1203,7 +1241,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3">
-        <v>44824</v>
+        <v>45291</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1224,7 +1262,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1242,13 +1280,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1260,27 +1298,45 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:1">

</xml_diff>